<commit_message>
Consider `u` for `Jumper`.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_jumper.xlsx
+++ b/andes/cases/ieee14/ieee14_jumper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuiha\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E99711E-DC28-461F-B820-D3728F600660}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD49B369-0451-423B-BF23-8D3CA8B0E783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8835" yWindow="480" windowWidth="21480" windowHeight="17355" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8835" yWindow="480" windowWidth="21480" windowHeight="17355" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="91">
   <si>
     <t>idx</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>J9-10</t>
+  </si>
+  <si>
+    <t>Line_12</t>
   </si>
 </sst>
 </file>
@@ -2358,11 +2361,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:X20"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3158,22 +3161,22 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="E13">
         <v>9</v>
       </c>
       <c r="F13">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G13">
         <v>100</v>
@@ -3188,10 +3191,10 @@
         <v>138</v>
       </c>
       <c r="K13">
-        <v>0.12711</v>
+        <v>3.1809999999999998E-2</v>
       </c>
       <c r="L13">
-        <v>0.27038000000000001</v>
+        <v>8.4500000000000006E-2</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -3223,22 +3226,22 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G14">
         <v>100</v>
@@ -3253,10 +3256,10 @@
         <v>138</v>
       </c>
       <c r="K14">
-        <v>8.2049999999999998E-2</v>
+        <v>0.12711</v>
       </c>
       <c r="L14">
-        <v>0.19206999999999999</v>
+        <v>0.27038000000000001</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -3288,22 +3291,22 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>100</v>
@@ -3318,10 +3321,10 @@
         <v>138</v>
       </c>
       <c r="K15">
-        <v>0.22092000000000001</v>
+        <v>8.2049999999999998E-2</v>
       </c>
       <c r="L15">
-        <v>0.19988</v>
+        <v>0.19206999999999999</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -3353,22 +3356,22 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16">
+        <v>12</v>
+      </c>
+      <c r="F16">
         <v>13</v>
-      </c>
-      <c r="F16">
-        <v>14</v>
       </c>
       <c r="G16">
         <v>100</v>
@@ -3383,10 +3386,10 @@
         <v>138</v>
       </c>
       <c r="K16">
-        <v>0.17093</v>
+        <v>0.22092000000000001</v>
       </c>
       <c r="L16">
-        <v>0.34802</v>
+        <v>0.19988</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -3418,22 +3421,22 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F17">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G17">
         <v>100</v>
@@ -3442,16 +3445,16 @@
         <v>60</v>
       </c>
       <c r="I17">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="J17">
         <v>138</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>0.17093</v>
       </c>
       <c r="L17">
-        <v>0.20912</v>
+        <v>0.34802</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -3472,10 +3475,10 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <v>0.99677000000000004</v>
+        <v>1</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -3483,22 +3486,22 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
       <c r="F18">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G18">
         <v>100</v>
@@ -3516,7 +3519,7 @@
         <v>0</v>
       </c>
       <c r="L18">
-        <v>0.55618000000000001</v>
+        <v>0.20912</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -3548,22 +3551,22 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G19">
         <v>100</v>
@@ -3572,16 +3575,16 @@
         <v>60</v>
       </c>
       <c r="I19">
-        <v>138</v>
+        <v>69</v>
       </c>
       <c r="J19">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>0.25202000000000002</v>
+        <v>0.55618000000000001</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -3613,22 +3616,22 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G20">
         <v>100</v>
@@ -3637,16 +3640,16 @@
         <v>60</v>
       </c>
       <c r="I20">
+        <v>138</v>
+      </c>
+      <c r="J20">
         <v>69</v>
       </c>
-      <c r="J20">
-        <v>138</v>
-      </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>0.17615</v>
+        <v>0.25202000000000002</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -3673,6 +3676,71 @@
         <v>0.99677000000000004</v>
       </c>
       <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="H21">
+        <v>60</v>
+      </c>
+      <c r="I21">
+        <v>69</v>
+      </c>
+      <c r="J21">
+        <v>138</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0.17615</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>0.99677000000000004</v>
+      </c>
+      <c r="U21">
         <v>0</v>
       </c>
     </row>
@@ -3743,9 +3811,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>